<commit_message>
Added graph with chart
</commit_message>
<xml_diff>
--- a/data/datos.xlsx
+++ b/data/datos.xlsx
@@ -1,47 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Hoja 1"/>
   </sheets>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Muestra</t>
+  </si>
+  <si>
+    <t>Observacion 1</t>
+  </si>
+  <si>
+    <t>Observacion 2</t>
+  </si>
+  <si>
+    <t>Observacion 3</t>
+  </si>
+  <si>
+    <t>Observacion 4</t>
+  </si>
+  <si>
+    <t>Observacion 5</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,7 +62,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -64,14 +81,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="5">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -80,10 +114,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -121,71 +155,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -209,50 +243,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -262,7 +299,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -271,7 +308,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -280,7 +317,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -288,10 +325,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -320,7 +357,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -333,13 +370,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -351,600 +387,559 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Muestra</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Observacion 1</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Observacion 2</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Observacion 3</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Observacion 4</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Observacion 5</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
         <v>74.03</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>74.002</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>74.019</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>73.992</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>74.008</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>73.995</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>73.992</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>74.001</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>74.011</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>74.004</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>73.998</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>74.024</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>74.021</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>74.005</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>74.002</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>74.002</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>73.996</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>73.993</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>74.015</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>74.009</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>73.992</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>74.007</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>74.015</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>73.989</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>74.014</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>74.009</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>73.994</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>73.997</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>73.985</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>73.993</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>73.995</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>74.006</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>73.994</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>74</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>74.005</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>73.985</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>74.003</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>73.993</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>74.015</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>73.988</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>74.008</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>73.995</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>74.009</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>74.005</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>74.004</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>73.998</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>74</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>73.99</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>74.007</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>73.995</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>73.994</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>73.998</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>73.994</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <v>73.995</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>73.99</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>74.004</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>74</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>74.007</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>74</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>73.996</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>73.983</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <v>74.002</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <v>73.998</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3">
         <v>73.997</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="3">
         <v>74.012</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>74.006</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>73.967</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>73.994</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>74</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="3">
         <v>73.984</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>74.012</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>74.014</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>73.998</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="3">
         <v>73.999</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <v>74.007</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>74</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="3">
         <v>73.984</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <v>74.005</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="3">
         <v>73.998</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <v>73.996</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>73.994</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="3">
         <v>74.012</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <v>73.986</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
         <v>74.005</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <v>74.007</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="3">
         <v>74.006</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="3">
         <v>74.01</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <v>74.018</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="3">
         <v>74.003</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="3">
         <v>73.984</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <v>74.002</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <v>74.003</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="3">
         <v>74.005</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>73.997</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>74</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <v>74.01</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <v>74.013</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="3">
         <v>74.02</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <v>74.003</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="3">
         <v>73.982</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="3">
         <v>74.001</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="3">
         <v>74.015</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="3">
         <v>74.005</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <v>73.996</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="3">
         <v>74.004</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
         <v>73.999</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <v>73.99</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="3">
         <v>74.006</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <v>74.009</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="3">
         <v>74.01</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
         <v>73.989</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="3">
         <v>73.99</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="3">
         <v>74.009</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="3">
         <v>74.014</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="3">
         <v>74.015</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3">
         <v>74.008</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="3">
         <v>73.993</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>74</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="3">
         <v>74.01</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="3">
         <v>73.982</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="3">
         <v>73.984</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="3">
         <v>73.995</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="3">
         <v>74.017</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3">
         <v>74.013</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27">
-        <v>3</v>
-      </c>
-      <c r="E27">
-        <v>4</v>
-      </c>
-      <c r="F27">
-        <v>5</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F27"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed values in samples and added button to delete the file
</commit_message>
<xml_diff>
--- a/data/datos.xlsx
+++ b/data/datos.xlsx
@@ -434,7 +434,7 @@
     <col min="11" max="11" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,7 +459,7 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -484,7 +484,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -509,7 +509,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -534,7 +534,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -559,7 +559,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -584,7 +584,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -609,7 +609,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -634,7 +634,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -659,7 +659,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -684,7 +684,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -709,7 +709,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -734,7 +734,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -759,7 +759,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -809,7 +809,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -834,7 +834,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -859,7 +859,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -884,7 +884,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -909,7 +909,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -934,7 +934,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -959,7 +959,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -984,7 +984,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1009,7 +1009,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -1034,7 +1034,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -1059,7 +1059,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1072,7 +1072,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1085,7 +1085,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1098,7 +1098,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1111,7 +1111,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1124,7 +1124,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1137,7 +1137,7 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1150,7 +1150,7 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1163,7 +1163,7 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -1176,7 +1176,7 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -1189,7 +1189,7 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1202,7 +1202,7 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1215,7 +1215,7 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -1228,7 +1228,7 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -1722,7 +1722,7 @@
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="17.25">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>

</xml_diff>